<commit_message>
ejercicio de async en java
apreciones suma y resta en dos hilos
</commit_message>
<xml_diff>
--- a/clean-code/Tests.xlsx
+++ b/clean-code/Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://personalsoftsas-my.sharepoint.com/personal/aegiraldo_personalsoft_com_co/Documents/Documentos/GitHub/AndresGiraldo/clean-code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{D6A1A21B-52B1-4106-85E9-D81887D81B82}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{2F9786B6-71D0-42EC-9BE1-1CA94399B7D8}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{D6A1A21B-52B1-4106-85E9-D81887D81B82}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{31ABB231-6718-41C6-B757-7AF7A5C90A4F}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BA33470E-338C-436F-BB18-0501D02584F7}"/>
   </bookViews>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
-  <si>
-    <t>Los libros se pueden prestar maximo por 1 mes y solo se pueden hacer renovaciones por una semana mas</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>entrada</t>
   </si>
@@ -36,49 +33,64 @@
     <t>salida</t>
   </si>
   <si>
-    <t>tiempo cumplido</t>
-  </si>
-  <si>
-    <t>Ampliacion del prestamo</t>
-  </si>
-  <si>
-    <t>tiempo cumplido sin devolucion</t>
-  </si>
-  <si>
-    <t>Notificacion Al usuario</t>
-  </si>
-  <si>
     <t>test</t>
   </si>
   <si>
     <t>ID del libro</t>
   </si>
   <si>
-    <t>ID del libro,Fecha de vencimiento</t>
-  </si>
-  <si>
-    <t>ID del libro, ID Usuario</t>
-  </si>
-  <si>
-    <t>Mensaje al ausuario que tiene libros sin entregar</t>
-  </si>
-  <si>
-    <t>Se actualiza el estado del prestamo del libro a disponible</t>
-  </si>
-  <si>
-    <t>Se actualiza la fecha de vencimiento a una seman mas y el estado del libro sigue en Ocupado</t>
-  </si>
-  <si>
-    <t>Se actualiza el estado del prestamo a ocupado con vencimiento</t>
-  </si>
-  <si>
-    <t>ID usuario</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Se guarda una sancion al usuario </t>
-  </si>
-  <si>
-    <t>Sanción</t>
+    <t>Los libros se pueden prestar maximo por 1 mes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">obtener tiemepo </t>
+  </si>
+  <si>
+    <t>esta vencido el libro</t>
+  </si>
+  <si>
+    <t>obtener el tiempo del prestamo</t>
+  </si>
+  <si>
+    <t>esta vigente el prestamo</t>
+  </si>
+  <si>
+    <t>numero de dias del libro</t>
+  </si>
+  <si>
+    <t>id del libro</t>
+  </si>
+  <si>
+    <t>fecha del libro</t>
+  </si>
+  <si>
+    <t>dias restantes</t>
+  </si>
+  <si>
+    <t>actualizar la fecha del libro</t>
+  </si>
+  <si>
+    <t>obtener disponibilidad del libro</t>
+  </si>
+  <si>
+    <t>buscar libro</t>
+  </si>
+  <si>
+    <t>solo se pueden prestar libros disponibles</t>
+  </si>
+  <si>
+    <t>guardar el prestamo del libro</t>
+  </si>
+  <si>
+    <t>libro ocupado</t>
+  </si>
+  <si>
+    <t>estado del libro</t>
+  </si>
+  <si>
+    <t>Se puede ampliar el plazo por una semana solicitandolo 2 dias antes</t>
+  </si>
+  <si>
+    <t>consultar disponibilidad de renovacion</t>
   </si>
 </sst>
 </file>
@@ -143,7 +155,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -152,6 +164,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -466,94 +479,134 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92BBDC36-8094-4998-A9AB-4A5F88E06B29}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="1" max="1" width="62.140625" customWidth="1"/>
     <col min="2" max="2" width="23.42578125" customWidth="1"/>
     <col min="3" max="3" width="33.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>1</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>16</v>
-      </c>
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>